<commit_message>
fix actuators quantity in bom
</commit_message>
<xml_diff>
--- a/智元灵犀X1_BOM清单_20241024.xlsx
+++ b/智元灵犀X1_BOM清单_20241024.xlsx
@@ -227,7 +227,7 @@
     <t>R52</t>
   </si>
   <si>
-    <t>R86</t>
+    <t>R86-2</t>
   </si>
   <si>
     <t>手臂_关节01固定法兰1</t>
@@ -2050,9 +2050,9 @@
   <dimension ref="A1:H339"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I187" sqref="I187"/>
+      <selection pane="bottomLeft" activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="25.2" customHeight="1" outlineLevelCol="7"/>
@@ -2510,7 +2510,7 @@
       <c r="G21" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H21" s="6" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2759,7 +2759,7 @@
         <v>19</v>
       </c>
       <c r="D34" s="5">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>11</v>
@@ -2777,7 +2777,7 @@
         <v>19</v>
       </c>
       <c r="D35" s="5">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>11</v>

</xml_diff>